<commit_message>
BF: TIDC update district list
</commit_message>
<xml_diff>
--- a/Coverage Survey/Burkina Faso/Oncho/Mai 2021/bf_ect_Oncho_1_village_202105.xlsx
+++ b/Coverage Survey/Burkina Faso/Oncho/Mai 2021/bf_ect_Oncho_1_village_202105.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repositories\WHO\dsa-forms\Coverage Survey\Burkina Faso\Oncho\Mai 2021\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA67206E-BCB7-4117-A68B-E0752E23DE7F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEBE2B0B-4946-4DF5-9DEA-DE1C3CAEA145}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="13986" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15360" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="81">
   <si>
     <t>type</t>
   </si>
@@ -262,6 +262,9 @@
   </si>
   <si>
     <t>ALIDOUGOU</t>
+  </si>
+  <si>
+    <t>LOGOGNEGUE 3</t>
   </si>
 </sst>
 </file>
@@ -649,7 +652,7 @@
   </sheetPr>
   <dimension ref="A1:H11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
@@ -847,11 +850,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:F54"/>
+  <dimension ref="A1:F56"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A55" sqref="A55:A64"/>
+      <selection pane="bottomLeft" activeCell="A46" sqref="A46:A47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1180,10 +1183,10 @@
         <v>44</v>
       </c>
       <c r="B25" t="s">
-        <v>71</v>
+        <v>80</v>
       </c>
       <c r="C25" t="s">
-        <v>71</v>
+        <v>80</v>
       </c>
       <c r="E25" t="s">
         <v>57</v>
@@ -1194,10 +1197,10 @@
         <v>44</v>
       </c>
       <c r="B26" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C26" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E26" t="s">
         <v>57</v>
@@ -1208,10 +1211,10 @@
         <v>44</v>
       </c>
       <c r="B27" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C27" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E27" t="s">
         <v>57</v>
@@ -1222,13 +1225,13 @@
         <v>44</v>
       </c>
       <c r="B28" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C28" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E28" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
@@ -1236,10 +1239,10 @@
         <v>44</v>
       </c>
       <c r="B29" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C29" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E29" t="s">
         <v>58</v>
@@ -1250,10 +1253,10 @@
         <v>44</v>
       </c>
       <c r="B30" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C30" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E30" t="s">
         <v>58</v>
@@ -1264,13 +1267,13 @@
         <v>44</v>
       </c>
       <c r="B31" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C31" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E31" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
@@ -1278,10 +1281,10 @@
         <v>44</v>
       </c>
       <c r="B32" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C32" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E32" t="s">
         <v>59</v>
@@ -1292,44 +1295,44 @@
         <v>44</v>
       </c>
       <c r="B33" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C33" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E33" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A34" s="2"/>
+      <c r="A34" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B34" t="s">
+        <v>79</v>
+      </c>
+      <c r="C34" t="s">
+        <v>79</v>
+      </c>
+      <c r="E34" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A35" t="s">
-        <v>48</v>
-      </c>
-      <c r="B35">
-        <v>1</v>
-      </c>
-      <c r="C35">
-        <v>1</v>
-      </c>
-      <c r="F35" t="s">
-        <v>60</v>
-      </c>
+      <c r="A35" s="2"/>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>48</v>
       </c>
       <c r="B36">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C36">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F36" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.2">
@@ -1337,13 +1340,13 @@
         <v>48</v>
       </c>
       <c r="B37">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C37">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F37" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.2">
@@ -1351,13 +1354,13 @@
         <v>48</v>
       </c>
       <c r="B38">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C38">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F38" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.2">
@@ -1365,13 +1368,13 @@
         <v>48</v>
       </c>
       <c r="B39">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C39">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F39" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.2">
@@ -1379,13 +1382,13 @@
         <v>48</v>
       </c>
       <c r="B40">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C40">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F40" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.2">
@@ -1393,13 +1396,13 @@
         <v>48</v>
       </c>
       <c r="B41">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C41">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F41" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.2">
@@ -1407,13 +1410,13 @@
         <v>48</v>
       </c>
       <c r="B42">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C42">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F42" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.2">
@@ -1421,13 +1424,13 @@
         <v>48</v>
       </c>
       <c r="B43">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C43">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F43" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.2">
@@ -1435,13 +1438,13 @@
         <v>48</v>
       </c>
       <c r="B44">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C44">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F44" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.2">
@@ -1449,13 +1452,13 @@
         <v>48</v>
       </c>
       <c r="B45">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C45">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F45" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.2">
@@ -1463,13 +1466,13 @@
         <v>48</v>
       </c>
       <c r="B46">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C46">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F46" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.2">
@@ -1477,13 +1480,13 @@
         <v>48</v>
       </c>
       <c r="B47">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C47">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F47" t="s">
-        <v>72</v>
+        <v>80</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.2">
@@ -1491,13 +1494,13 @@
         <v>48</v>
       </c>
       <c r="B48">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C48">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F48" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.2">
@@ -1505,13 +1508,13 @@
         <v>48</v>
       </c>
       <c r="B49">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C49">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F49" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.2">
@@ -1519,13 +1522,13 @@
         <v>48</v>
       </c>
       <c r="B50">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C50">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F50" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.2">
@@ -1533,13 +1536,13 @@
         <v>48</v>
       </c>
       <c r="B51">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C51">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F51" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.2">
@@ -1547,13 +1550,13 @@
         <v>48</v>
       </c>
       <c r="B52">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C52">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F52" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.2">
@@ -1561,13 +1564,13 @@
         <v>48</v>
       </c>
       <c r="B53">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C53">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F53" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.2">
@@ -1575,12 +1578,40 @@
         <v>48</v>
       </c>
       <c r="B54">
+        <v>19</v>
+      </c>
+      <c r="C54">
+        <v>19</v>
+      </c>
+      <c r="F54" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
+        <v>48</v>
+      </c>
+      <c r="B55">
         <v>20</v>
       </c>
-      <c r="C54">
+      <c r="C55">
         <v>20</v>
       </c>
-      <c r="F54" t="s">
+      <c r="F55" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
+        <v>48</v>
+      </c>
+      <c r="B56">
+        <v>21</v>
+      </c>
+      <c r="C56">
+        <v>21</v>
+      </c>
+      <c r="F56" t="s">
         <v>79</v>
       </c>
     </row>
@@ -1602,7 +1633,7 @@
   </sheetPr>
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
BF: TIDC may 2021 update site liste
</commit_message>
<xml_diff>
--- a/Coverage Survey/Burkina Faso/Oncho/Mai 2021/bf_ect_Oncho_1_village_202105.xlsx
+++ b/Coverage Survey/Burkina Faso/Oncho/Mai 2021/bf_ect_Oncho_1_village_202105.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repositories\WHO\dsa-forms\Coverage Survey\Burkina Faso\Oncho\Mai 2021\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEBE2B0B-4946-4DF5-9DEA-DE1C3CAEA145}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E63823C-BE67-4F13-BB93-C3D4E8C60456}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15360" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="105">
   <si>
     <t>type</t>
   </si>
@@ -225,9 +225,6 @@
     <t>SENEKO</t>
   </si>
   <si>
-    <t>TIEKELEDOUGOU</t>
-  </si>
-  <si>
     <t>CAMP MARABOUT</t>
   </si>
   <si>
@@ -237,15 +234,6 @@
     <t>LOGOGNEGUE 2</t>
   </si>
   <si>
-    <t>LAWORO 1</t>
-  </si>
-  <si>
-    <t>LAWORO 2</t>
-  </si>
-  <si>
-    <t>LAWORO 3</t>
-  </si>
-  <si>
     <t>GNAGNA</t>
   </si>
   <si>
@@ -265,6 +253,90 @@
   </si>
   <si>
     <t>LOGOGNEGUE 3</t>
+  </si>
+  <si>
+    <t>SIRAKORO</t>
+  </si>
+  <si>
+    <t>SOKOURA3</t>
+  </si>
+  <si>
+    <t>SOKOURA4</t>
+  </si>
+  <si>
+    <t>THIONIDOUGOU+LIMITEDOUGOU</t>
+  </si>
+  <si>
+    <t>LAWORO</t>
+  </si>
+  <si>
+    <t>TIEKELEDOUGOU 1</t>
+  </si>
+  <si>
+    <t>TIEKELEDOUGOU 2</t>
+  </si>
+  <si>
+    <t>5 </t>
+  </si>
+  <si>
+    <t>2 </t>
+  </si>
+  <si>
+    <t>3 </t>
+  </si>
+  <si>
+    <t>4 </t>
+  </si>
+  <si>
+    <t>1 </t>
+  </si>
+  <si>
+    <t>19 </t>
+  </si>
+  <si>
+    <t>18 </t>
+  </si>
+  <si>
+    <t>20 </t>
+  </si>
+  <si>
+    <t>21 </t>
+  </si>
+  <si>
+    <t>15 </t>
+  </si>
+  <si>
+    <t>16 </t>
+  </si>
+  <si>
+    <t>17 </t>
+  </si>
+  <si>
+    <t>14 </t>
+  </si>
+  <si>
+    <t>11 </t>
+  </si>
+  <si>
+    <t>12 </t>
+  </si>
+  <si>
+    <t>13 </t>
+  </si>
+  <si>
+    <t>6 </t>
+  </si>
+  <si>
+    <t>10 </t>
+  </si>
+  <si>
+    <t>7 </t>
+  </si>
+  <si>
+    <t>8 </t>
+  </si>
+  <si>
+    <t>9 </t>
   </si>
 </sst>
 </file>
@@ -850,11 +922,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:F56"/>
+  <dimension ref="A1:F59"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A46" sqref="A46:A47"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F39" sqref="F39:F59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -970,10 +1042,10 @@
         <v>34</v>
       </c>
       <c r="B9" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="C9" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>54</v>
@@ -984,10 +1056,10 @@
         <v>34</v>
       </c>
       <c r="B10" t="s">
-        <v>57</v>
+        <v>77</v>
       </c>
       <c r="C10" t="s">
-        <v>57</v>
+        <v>77</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>54</v>
@@ -1012,69 +1084,70 @@
         <v>34</v>
       </c>
       <c r="B12" t="s">
-        <v>59</v>
+        <v>78</v>
       </c>
       <c r="C12" t="s">
-        <v>59</v>
+        <v>78</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A13" s="2"/>
+      <c r="A13" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B13" t="s">
+        <v>79</v>
+      </c>
+      <c r="C13" t="s">
+        <v>79</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="B14" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C14" t="s">
-        <v>60</v>
-      </c>
-      <c r="E14" t="s">
-        <v>55</v>
+        <v>57</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="B15" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="C15" t="s">
-        <v>61</v>
-      </c>
-      <c r="E15" t="s">
-        <v>55</v>
+        <v>56</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A16" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="B16" t="s">
-        <v>62</v>
-      </c>
-      <c r="C16" t="s">
-        <v>62</v>
-      </c>
-      <c r="E16" t="s">
-        <v>55</v>
-      </c>
+      <c r="A16" s="2"/>
+      <c r="D16" s="2"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
         <v>44</v>
       </c>
       <c r="B17" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C17" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="E17" t="s">
         <v>55</v>
@@ -1085,10 +1158,10 @@
         <v>44</v>
       </c>
       <c r="B18" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C18" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="E18" t="s">
         <v>55</v>
@@ -1099,13 +1172,13 @@
         <v>44</v>
       </c>
       <c r="B19" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C19" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="E19" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
@@ -1113,13 +1186,13 @@
         <v>44</v>
       </c>
       <c r="B20" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C20" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="E20" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
@@ -1127,41 +1200,41 @@
         <v>44</v>
       </c>
       <c r="B21" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="C21" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="E21" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="B22" s="8" t="s">
-        <v>68</v>
+      <c r="B22" t="s">
+        <v>74</v>
       </c>
       <c r="C22" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="E22" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="B23" s="8" t="s">
-        <v>69</v>
+      <c r="B23" t="s">
+        <v>73</v>
       </c>
       <c r="C23" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="E23" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
@@ -1169,41 +1242,41 @@
         <v>44</v>
       </c>
       <c r="B24" t="s">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="C24" t="s">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="E24" t="s">
-        <v>57</v>
+        <v>77</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B25" s="8" t="s">
         <v>80</v>
       </c>
       <c r="C25" t="s">
         <v>80</v>
       </c>
       <c r="E25" t="s">
-        <v>57</v>
+        <v>77</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="B26" t="s">
-        <v>71</v>
+      <c r="B26" s="8" t="s">
+        <v>70</v>
       </c>
       <c r="C26" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E26" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
@@ -1211,13 +1284,13 @@
         <v>44</v>
       </c>
       <c r="B27" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C27" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E27" t="s">
-        <v>57</v>
+        <v>78</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
@@ -1225,13 +1298,13 @@
         <v>44</v>
       </c>
       <c r="B28" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C28" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E28" t="s">
-        <v>57</v>
+        <v>79</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
@@ -1239,13 +1312,13 @@
         <v>44</v>
       </c>
       <c r="B29" t="s">
-        <v>74</v>
+        <v>81</v>
       </c>
       <c r="C29" t="s">
-        <v>74</v>
+        <v>81</v>
       </c>
       <c r="E29" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
@@ -1253,13 +1326,13 @@
         <v>44</v>
       </c>
       <c r="B30" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="C30" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="E30" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
@@ -1267,13 +1340,13 @@
         <v>44</v>
       </c>
       <c r="B31" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="C31" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="E31" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
@@ -1281,13 +1354,13 @@
         <v>44</v>
       </c>
       <c r="B32" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C32" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E32" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.2">
@@ -1295,13 +1368,13 @@
         <v>44</v>
       </c>
       <c r="B33" t="s">
-        <v>78</v>
+        <v>65</v>
       </c>
       <c r="C33" t="s">
-        <v>78</v>
+        <v>65</v>
       </c>
       <c r="E33" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.2">
@@ -1309,181 +1382,181 @@
         <v>44</v>
       </c>
       <c r="B34" t="s">
-        <v>79</v>
+        <v>67</v>
       </c>
       <c r="C34" t="s">
-        <v>79</v>
+        <v>67</v>
       </c>
       <c r="E34" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A35" s="2"/>
+      <c r="A35" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B35" t="s">
+        <v>66</v>
+      </c>
+      <c r="C35" t="s">
+        <v>66</v>
+      </c>
+      <c r="E35" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A36" t="s">
-        <v>48</v>
-      </c>
-      <c r="B36">
-        <v>1</v>
-      </c>
-      <c r="C36">
-        <v>1</v>
-      </c>
-      <c r="F36" t="s">
-        <v>60</v>
+      <c r="A36" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B36" t="s">
+        <v>82</v>
+      </c>
+      <c r="C36" t="s">
+        <v>82</v>
+      </c>
+      <c r="E36" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A37" t="s">
-        <v>48</v>
-      </c>
-      <c r="B37">
-        <v>2</v>
-      </c>
-      <c r="C37">
-        <v>2</v>
-      </c>
-      <c r="F37" t="s">
-        <v>61</v>
+      <c r="A37" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B37" t="s">
+        <v>83</v>
+      </c>
+      <c r="C37" t="s">
+        <v>83</v>
+      </c>
+      <c r="E37" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A38" t="s">
-        <v>48</v>
-      </c>
-      <c r="B38">
-        <v>3</v>
-      </c>
-      <c r="C38">
-        <v>3</v>
-      </c>
-      <c r="F38" t="s">
-        <v>62</v>
-      </c>
+      <c r="A38" s="2"/>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>48</v>
       </c>
-      <c r="B39">
-        <v>4</v>
-      </c>
-      <c r="C39">
-        <v>4</v>
+      <c r="B39" t="s">
+        <v>84</v>
+      </c>
+      <c r="C39" t="s">
+        <v>84</v>
       </c>
       <c r="F39" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>48</v>
       </c>
-      <c r="B40">
-        <v>5</v>
-      </c>
-      <c r="C40">
-        <v>5</v>
+      <c r="B40" t="s">
+        <v>85</v>
+      </c>
+      <c r="C40" t="s">
+        <v>85</v>
       </c>
       <c r="F40" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>48</v>
       </c>
-      <c r="B41">
-        <v>6</v>
-      </c>
-      <c r="C41">
-        <v>6</v>
+      <c r="B41" t="s">
+        <v>86</v>
+      </c>
+      <c r="C41" t="s">
+        <v>86</v>
       </c>
       <c r="F41" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>48</v>
       </c>
-      <c r="B42">
-        <v>7</v>
-      </c>
-      <c r="C42">
-        <v>7</v>
+      <c r="B42" t="s">
+        <v>87</v>
+      </c>
+      <c r="C42" t="s">
+        <v>87</v>
       </c>
       <c r="F42" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>48</v>
       </c>
-      <c r="B43">
-        <v>8</v>
-      </c>
-      <c r="C43">
-        <v>8</v>
+      <c r="B43" t="s">
+        <v>88</v>
+      </c>
+      <c r="C43" t="s">
+        <v>88</v>
       </c>
       <c r="F43" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>48</v>
       </c>
-      <c r="B44">
-        <v>9</v>
-      </c>
-      <c r="C44">
-        <v>9</v>
+      <c r="B44" t="s">
+        <v>89</v>
+      </c>
+      <c r="C44" t="s">
+        <v>89</v>
       </c>
       <c r="F44" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>48</v>
       </c>
-      <c r="B45">
-        <v>10</v>
-      </c>
-      <c r="C45">
-        <v>10</v>
+      <c r="B45" t="s">
+        <v>90</v>
+      </c>
+      <c r="C45" t="s">
+        <v>90</v>
       </c>
       <c r="F45" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>48</v>
       </c>
-      <c r="B46">
-        <v>11</v>
-      </c>
-      <c r="C46">
-        <v>11</v>
+      <c r="B46" t="s">
+        <v>91</v>
+      </c>
+      <c r="C46" t="s">
+        <v>91</v>
       </c>
       <c r="F46" t="s">
-        <v>70</v>
+        <v>75</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>48</v>
       </c>
-      <c r="B47">
-        <v>12</v>
-      </c>
-      <c r="C47">
-        <v>12</v>
+      <c r="B47" t="s">
+        <v>92</v>
+      </c>
+      <c r="C47" t="s">
+        <v>92</v>
       </c>
       <c r="F47" t="s">
         <v>80</v>
@@ -1493,126 +1566,168 @@
       <c r="A48" t="s">
         <v>48</v>
       </c>
-      <c r="B48">
-        <v>13</v>
-      </c>
-      <c r="C48">
-        <v>13</v>
+      <c r="B48" t="s">
+        <v>93</v>
+      </c>
+      <c r="C48" t="s">
+        <v>93</v>
       </c>
       <c r="F48" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>48</v>
       </c>
-      <c r="B49">
-        <v>14</v>
-      </c>
-      <c r="C49">
-        <v>14</v>
+      <c r="B49" t="s">
+        <v>94</v>
+      </c>
+      <c r="C49" t="s">
+        <v>94</v>
       </c>
       <c r="F49" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>48</v>
       </c>
-      <c r="B50">
-        <v>15</v>
-      </c>
-      <c r="C50">
-        <v>15</v>
+      <c r="B50" t="s">
+        <v>95</v>
+      </c>
+      <c r="C50" t="s">
+        <v>95</v>
       </c>
       <c r="F50" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>48</v>
       </c>
-      <c r="B51">
-        <v>16</v>
-      </c>
-      <c r="C51">
-        <v>16</v>
+      <c r="B51" t="s">
+        <v>96</v>
+      </c>
+      <c r="C51" t="s">
+        <v>96</v>
       </c>
       <c r="F51" t="s">
-        <v>74</v>
+        <v>81</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>48</v>
       </c>
-      <c r="B52">
-        <v>17</v>
-      </c>
-      <c r="C52">
-        <v>17</v>
+      <c r="B52" t="s">
+        <v>97</v>
+      </c>
+      <c r="C52" t="s">
+        <v>97</v>
       </c>
       <c r="F52" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>48</v>
       </c>
-      <c r="B53">
-        <v>18</v>
-      </c>
-      <c r="C53">
-        <v>18</v>
+      <c r="B53" t="s">
+        <v>98</v>
+      </c>
+      <c r="C53" t="s">
+        <v>98</v>
       </c>
       <c r="F53" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>48</v>
       </c>
-      <c r="B54">
-        <v>19</v>
-      </c>
-      <c r="C54">
-        <v>19</v>
+      <c r="B54" t="s">
+        <v>99</v>
+      </c>
+      <c r="C54" t="s">
+        <v>99</v>
       </c>
       <c r="F54" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>48</v>
       </c>
-      <c r="B55">
-        <v>20</v>
-      </c>
-      <c r="C55">
-        <v>20</v>
+      <c r="B55" t="s">
+        <v>100</v>
+      </c>
+      <c r="C55" t="s">
+        <v>100</v>
       </c>
       <c r="F55" t="s">
-        <v>78</v>
+        <v>65</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>48</v>
       </c>
-      <c r="B56">
-        <v>21</v>
-      </c>
-      <c r="C56">
-        <v>21</v>
+      <c r="B56" t="s">
+        <v>101</v>
+      </c>
+      <c r="C56" t="s">
+        <v>101</v>
       </c>
       <c r="F56" t="s">
-        <v>79</v>
+        <v>67</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
+        <v>48</v>
+      </c>
+      <c r="B57" t="s">
+        <v>102</v>
+      </c>
+      <c r="C57" t="s">
+        <v>102</v>
+      </c>
+      <c r="F57" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
+        <v>48</v>
+      </c>
+      <c r="B58" t="s">
+        <v>103</v>
+      </c>
+      <c r="C58" t="s">
+        <v>103</v>
+      </c>
+      <c r="F58" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
+        <v>48</v>
+      </c>
+      <c r="B59" t="s">
+        <v>104</v>
+      </c>
+      <c r="C59" t="s">
+        <v>104</v>
+      </c>
+      <c r="F59" t="s">
+        <v>83</v>
       </c>
     </row>
   </sheetData>
@@ -1633,7 +1748,7 @@
   </sheetPr>
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>

</xml_diff>